<commit_message>
parse and print pearson class
</commit_message>
<xml_diff>
--- a/kontakty.xlsx
+++ b/kontakty.xlsx
@@ -22,13 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">Wspólnota 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adres</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t xml:space="preserve">Kowalski Jakub</t>
   </si>
@@ -101,7 +95,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -131,12 +125,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="12"/>
       <color rgb="FF0066CC"/>
@@ -145,11 +133,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color rgb="FF0066CC"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,26 +147,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -215,16 +188,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,31 +213,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -280,315 +241,295 @@
   <dimension ref="A1:O65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.8520408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="9.74489795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.71938775510204"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="9.74489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="18.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.9132653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="19.765306122449"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="C1" s="3" t="n">
+        <v>111111111</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="n">
-        <v>111111111</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="3" t="n">
+        <v>222222222</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="n">
-        <v>222222222</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="3" t="n">
+        <v>333333333</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="n">
-        <v>333333333</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="3" t="n">
+        <v>444444444</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="n">
-        <v>444444444</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="3" t="n">
+        <v>555555555</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="n">
-        <v>555555555</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="3" t="n">
+        <v>666666666</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="n">
-        <v>666666666</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="3" t="n">
+        <v>777777777</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="n">
-        <v>777777777</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="3" t="n">
+        <v>888888888</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="n">
-        <v>888888888</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="3" t="n">
+        <v>999999999</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="n">
-        <v>999999999</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="3" t="n">
+        <v>101010101</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>101010101</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -677,10 +618,10 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="adres@email.com"/>
-    <hyperlink ref="D5" r:id="rId2" display="adres@email.com"/>
-    <hyperlink ref="D7" r:id="rId3" display="adres@email.com"/>
-    <hyperlink ref="D9" r:id="rId4" display="adres@email.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="adres@email.com"/>
+    <hyperlink ref="D4" r:id="rId2" display="adres@email.com"/>
+    <hyperlink ref="D6" r:id="rId3" display="adres@email.com"/>
+    <hyperlink ref="D8" r:id="rId4" display="adres@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -705,8 +646,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="18.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.24489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="19.765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -753,8 +694,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="18.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.24489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="19.765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>